<commit_message>
Corrections fonctions de recherche
</commit_message>
<xml_diff>
--- a/FonctionsDeRecherche.xlsx
+++ b/FonctionsDeRecherche.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="557" activeTab="3"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="557" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="RECHERCHEV" sheetId="9882" r:id="rId1"/>
@@ -49,21 +49,15 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="213">
   <si>
     <t>Frais transport</t>
   </si>
   <si>
-    <t>De 0 à 5 614 €</t>
-  </si>
-  <si>
     <t>De 5 614 à 11 198 €</t>
   </si>
   <si>
     <t>De 11 199 à 24 872 €</t>
-  </si>
-  <si>
-    <t>De 24 873 à 66 679 €</t>
   </si>
   <si>
     <t>Au-delà de 66 679 €</t>
@@ -729,6 +723,15 @@
   </si>
   <si>
     <t>Remise</t>
+  </si>
+  <si>
+    <t>Pour savoir si un commercial est économe, on s'intéresse à ses dépenses en déplacement, et pour connaitre sa performance on regarde son chiffre d'affaires (CA).</t>
+  </si>
+  <si>
+    <t>De 0 à 5 613 €</t>
+  </si>
+  <si>
+    <t>De 24 873 à 66 678 €</t>
   </si>
 </sst>
 </file>
@@ -1763,13 +1766,13 @@
     <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>781050</xdr:colOff>
-      <xdr:row>4</xdr:row>
+      <xdr:row>5</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>12</xdr:col>
       <xdr:colOff>467442</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>23</xdr:row>
       <xdr:rowOff>114747</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -3076,77 +3079,77 @@
   <sheetData>
     <row r="1" spans="1:7" s="62" customFormat="1" ht="32.25" customHeight="1">
       <c r="A1" s="61" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="3" spans="1:7" s="62" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="135" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="24" customHeight="1">
       <c r="B5" s="66" t="s">
+        <v>191</v>
+      </c>
+      <c r="C5" s="66" t="s">
+        <v>192</v>
+      </c>
+      <c r="D5" s="66" t="s">
         <v>193</v>
-      </c>
-      <c r="C5" s="66" t="s">
-        <v>194</v>
-      </c>
-      <c r="D5" s="66" t="s">
-        <v>195</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25">
       <c r="B6" s="139" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" s="132" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D6" s="133">
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1">
       <c r="B7" s="139" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C7" s="132" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="D7" s="133">
         <v>4</v>
       </c>
       <c r="F7" s="66" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="G7" s="48" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1">
       <c r="B8" s="139" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C8" s="132" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D8" s="133">
         <v>5</v>
       </c>
       <c r="F8" s="66" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="G8" s="136"/>
     </row>
     <row r="9" spans="1:7" ht="14.25">
       <c r="B9" s="139" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C9" s="132" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D9" s="133">
         <v>3</v>
@@ -3154,10 +3157,10 @@
     </row>
     <row r="10" spans="1:7" ht="14.25">
       <c r="B10" s="139" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C10" s="132" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="D10" s="133">
         <v>7</v>
@@ -3165,10 +3168,10 @@
     </row>
     <row r="11" spans="1:7" ht="14.25">
       <c r="B11" s="139" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C11" s="132" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D11" s="133">
         <v>2</v>
@@ -3176,35 +3179,35 @@
     </row>
     <row r="15" spans="1:7" s="62" customFormat="1" ht="19.5" customHeight="1">
       <c r="A15" s="135" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
     </row>
     <row r="17" spans="2:8">
       <c r="B17" s="45" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="18" spans="2:8" ht="30">
       <c r="B18" s="66" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C18" s="66" t="s">
+        <v>182</v>
+      </c>
+      <c r="D18" s="66" t="s">
         <v>184</v>
-      </c>
-      <c r="D18" s="66" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="19" spans="2:8" ht="15">
       <c r="B19" s="54" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C19" s="134"/>
       <c r="D19" s="133">
         <v>15</v>
       </c>
       <c r="F19" s="66" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="G19" s="48">
         <v>150</v>
@@ -3213,20 +3216,20 @@
     </row>
     <row r="20" spans="2:8" ht="15">
       <c r="B20" s="54" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C20" s="134"/>
       <c r="D20" s="133">
         <v>25</v>
       </c>
       <c r="F20" s="66" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G20" s="137"/>
     </row>
     <row r="21" spans="2:8" ht="14.25">
       <c r="B21" s="54" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C21" s="134"/>
       <c r="D21" s="133">
@@ -3235,14 +3238,14 @@
     </row>
     <row r="22" spans="2:8" ht="15">
       <c r="B22" s="54" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C22" s="134"/>
       <c r="D22" s="133">
         <v>120</v>
       </c>
       <c r="F22" s="138" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -3274,7 +3277,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="62" customFormat="1" ht="32.25" customHeight="1">
       <c r="A1" s="61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C1" s="39"/>
       <c r="G1" s="39"/>
@@ -3282,28 +3285,28 @@
     <row r="2" spans="1:15" s="62" customFormat="1" ht="24" customHeight="1">
       <c r="A2" s="87"/>
       <c r="B2" s="97" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="G2" s="39"/>
       <c r="M2" s="46"/>
     </row>
     <row r="3" spans="1:15" ht="15">
       <c r="B3" s="97" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C3" s="4"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:15" ht="15">
       <c r="B4" s="97" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C4" s="4"/>
       <c r="G4" s="3"/>
     </row>
     <row r="5" spans="1:15" ht="15">
       <c r="B5" s="97" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C5" s="4"/>
       <c r="G5" s="3"/>
@@ -3315,7 +3318,7 @@
     </row>
     <row r="7" spans="1:15" ht="21" customHeight="1">
       <c r="B7" s="144" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="C7" s="145"/>
       <c r="D7" s="145"/>
@@ -3324,19 +3327,19 @@
     </row>
     <row r="8" spans="1:15" ht="23.25" customHeight="1">
       <c r="B8" s="66" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="C8" s="66" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D8" s="66" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E8" s="66" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="F8" s="66" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:15" ht="16.5" customHeight="1">
@@ -3408,7 +3411,7 @@
     <row r="16" spans="1:15" ht="21" customHeight="1">
       <c r="B16" s="3"/>
       <c r="E16" s="110" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="F16" s="99"/>
     </row>
@@ -3417,25 +3420,25 @@
     </row>
     <row r="18" spans="2:6" ht="17.25" customHeight="1">
       <c r="E18" s="100" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F18" s="111"/>
     </row>
     <row r="19" spans="2:6" ht="17.25" customHeight="1">
       <c r="E19" s="100" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F19" s="111"/>
     </row>
     <row r="20" spans="2:6" ht="17.25" customHeight="1">
       <c r="E20" s="100" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F20" s="111"/>
     </row>
     <row r="21" spans="2:6" ht="17.25" customHeight="1">
       <c r="E21" s="100" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F21" s="112">
         <v>0.2</v>
@@ -3443,13 +3446,13 @@
     </row>
     <row r="22" spans="2:6" ht="17.25" customHeight="1">
       <c r="E22" s="100" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F22" s="111"/>
     </row>
     <row r="23" spans="2:6" ht="18.75" customHeight="1">
       <c r="E23" s="100" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F23" s="99"/>
     </row>
@@ -3492,20 +3495,20 @@
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1">
       <c r="B2" s="144" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C2" s="145"/>
       <c r="D2" s="146"/>
     </row>
     <row r="3" spans="1:13" ht="27.75" customHeight="1">
       <c r="B3" s="66" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="C3" s="66" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D3" s="66" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="39" customFormat="1" ht="25.5" customHeight="1">
@@ -3513,7 +3516,7 @@
         <v>100</v>
       </c>
       <c r="C4" s="75" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D4" s="75">
         <v>15.21</v>
@@ -3524,7 +3527,7 @@
         <v>101</v>
       </c>
       <c r="C5" s="75" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D5" s="75">
         <v>14.63</v>
@@ -3535,7 +3538,7 @@
         <v>102</v>
       </c>
       <c r="C6" s="75" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="D6" s="75">
         <v>18.45</v>
@@ -3546,7 +3549,7 @@
         <v>103</v>
       </c>
       <c r="C7" s="75" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="D7" s="75">
         <v>19.989999999999998</v>
@@ -3557,7 +3560,7 @@
         <v>104</v>
       </c>
       <c r="C8" s="75" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D8" s="75">
         <v>16.21</v>
@@ -3568,7 +3571,7 @@
         <v>105</v>
       </c>
       <c r="C9" s="75" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="D9" s="75">
         <v>15.6</v>
@@ -3579,7 +3582,7 @@
         <v>106</v>
       </c>
       <c r="C10" s="75" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D10" s="75">
         <v>18.98</v>
@@ -3624,7 +3627,7 @@
   <sheetData>
     <row r="1" spans="1:17" s="62" customFormat="1" ht="32.25" customHeight="1">
       <c r="A1" s="61" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C1" s="39"/>
       <c r="G1" s="39"/>
@@ -3632,7 +3635,7 @@
     <row r="2" spans="1:17" s="62" customFormat="1" ht="24" customHeight="1">
       <c r="A2" s="87"/>
       <c r="B2" s="97" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="G2" s="39"/>
       <c r="M2" s="46"/>
@@ -3652,7 +3655,7 @@
     </row>
     <row r="4" spans="1:17" ht="21.75" customHeight="1">
       <c r="B4" s="142" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="C4" s="143"/>
       <c r="D4" s="143"/>
@@ -3666,7 +3669,7 @@
     <row r="5" spans="1:17" ht="21.75" customHeight="1">
       <c r="B5" s="27"/>
       <c r="C5" s="113" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D5" s="28"/>
       <c r="E5" s="131"/>
@@ -3679,7 +3682,7 @@
     <row r="6" spans="1:17" ht="21.75" customHeight="1">
       <c r="B6" s="27"/>
       <c r="C6" s="113" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D6" s="28"/>
       <c r="E6" s="131"/>
@@ -3703,7 +3706,7 @@
     <row r="8" spans="1:17" ht="21.75" customHeight="1">
       <c r="B8" s="27"/>
       <c r="C8" s="148" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="D8" s="148"/>
       <c r="E8" s="130"/>
@@ -3715,7 +3718,7 @@
     </row>
     <row r="9" spans="1:17" ht="16.5" customHeight="1" thickBot="1">
       <c r="H9" s="123" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="I9" s="122"/>
       <c r="J9" s="122"/>
@@ -3724,19 +3727,19 @@
     </row>
     <row r="10" spans="1:17" ht="29.25" customHeight="1">
       <c r="I10" s="121" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="J10" s="66" t="s">
+        <v>9</v>
+      </c>
+      <c r="K10" s="66" t="s">
+        <v>10</v>
+      </c>
+      <c r="L10" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="K10" s="66" t="s">
+      <c r="M10" s="66" t="s">
         <v>12</v>
-      </c>
-      <c r="L10" s="66" t="s">
-        <v>13</v>
-      </c>
-      <c r="M10" s="66" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="11" spans="1:17" ht="15" customHeight="1">
@@ -3838,7 +3841,7 @@
     <row r="18" spans="2:12" ht="16.5" thickBot="1">
       <c r="B18" s="26"/>
       <c r="H18" s="123" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="I18" s="36"/>
       <c r="J18" s="36"/>
@@ -3848,10 +3851,10 @@
     <row r="19" spans="2:12" ht="25.5" customHeight="1">
       <c r="B19" s="26"/>
       <c r="I19" s="124" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="J19" s="125" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="K19" s="36"/>
       <c r="L19" s="2"/>
@@ -3927,7 +3930,7 @@
   <sheetPr published="0"/>
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
@@ -3941,7 +3944,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="62" customFormat="1" ht="32.25" customHeight="1">
       <c r="A1" s="61" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -3949,17 +3952,17 @@
     </row>
     <row r="3" spans="1:15" s="62" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="135" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="97" customFormat="1" ht="14.25">
       <c r="A4" s="97" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="21" customHeight="1">
       <c r="B6" s="141" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="C6" s="49"/>
       <c r="D6" s="49"/>
@@ -3970,82 +3973,82 @@
       <c r="I6" s="49"/>
       <c r="J6" s="49"/>
       <c r="M6" s="66" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="N6" s="66" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="O6" s="66" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
     </row>
     <row r="7" spans="1:15" ht="21" customHeight="1">
       <c r="B7" s="66" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C7" s="139" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="139" t="s">
         <v>46</v>
       </c>
-      <c r="D7" s="139" t="s">
+      <c r="E7" s="139" t="s">
         <v>48</v>
       </c>
-      <c r="E7" s="139" t="s">
+      <c r="F7" s="139" t="s">
         <v>50</v>
       </c>
-      <c r="F7" s="139" t="s">
-        <v>52</v>
-      </c>
       <c r="G7" s="139" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="H7" s="139" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="I7" s="48" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="J7" s="48" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="M7" s="139" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="N7" s="134"/>
       <c r="O7" s="140"/>
     </row>
     <row r="8" spans="1:15" ht="21" customHeight="1">
       <c r="B8" s="66" t="s">
+        <v>192</v>
+      </c>
+      <c r="C8" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="C8" s="48" t="s">
+      <c r="D8" s="48" t="s">
+        <v>195</v>
+      </c>
+      <c r="E8" s="48" t="s">
         <v>196</v>
       </c>
-      <c r="D8" s="48" t="s">
+      <c r="F8" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="E8" s="48" t="s">
-        <v>198</v>
-      </c>
-      <c r="F8" s="48" t="s">
-        <v>199</v>
-      </c>
       <c r="G8" s="48" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="H8" s="48" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="I8" s="48" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="J8" s="48" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="M8" s="45"/>
     </row>
     <row r="9" spans="1:15" ht="21" customHeight="1">
       <c r="B9" s="66" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C9" s="48">
         <v>12</v>
@@ -4083,7 +4086,7 @@
   <dimension ref="A1:M21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -4101,19 +4104,19 @@
   <sheetData>
     <row r="1" spans="1:13" s="62" customFormat="1" ht="32.25" customHeight="1">
       <c r="A1" s="61" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="62" customFormat="1" ht="24" customHeight="1">
       <c r="A2" s="61"/>
       <c r="B2" s="63" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="M2" s="46"/>
     </row>
     <row r="3" spans="1:13" s="64" customFormat="1">
       <c r="B3" s="63" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="D3" s="65"/>
     </row>
@@ -4123,22 +4126,22 @@
     </row>
     <row r="5" spans="1:13" ht="15">
       <c r="B5" s="66" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="D5" s="66" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="E5" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="I5" s="66" t="s">
         <v>121</v>
       </c>
-      <c r="I5" s="66" t="s">
-        <v>123</v>
-      </c>
       <c r="J5" s="66" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="15.75" customHeight="1">
@@ -4146,16 +4149,16 @@
         <v>1</v>
       </c>
       <c r="C6" s="67" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D6" s="68" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="E6" s="69">
         <v>23235</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>1</v>
+        <v>211</v>
       </c>
       <c r="I6" s="72"/>
       <c r="J6" s="73">
@@ -4167,16 +4170,16 @@
         <v>2</v>
       </c>
       <c r="C7" s="67" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D7" s="68" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E7" s="69">
         <v>28656</v>
       </c>
       <c r="H7" s="37" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="I7" s="72"/>
       <c r="J7" s="73">
@@ -4188,16 +4191,16 @@
         <v>3</v>
       </c>
       <c r="C8" s="67" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" s="68" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E8" s="69">
         <v>27142</v>
       </c>
       <c r="H8" s="37" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="I8" s="72"/>
       <c r="J8" s="73">
@@ -4209,16 +4212,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="67" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D9" s="68" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E9" s="69">
         <v>23483</v>
       </c>
       <c r="H9" s="37" t="s">
-        <v>4</v>
+        <v>212</v>
       </c>
       <c r="I9" s="72"/>
       <c r="J9" s="73">
@@ -4230,16 +4233,16 @@
         <v>5</v>
       </c>
       <c r="C10" s="67" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D10" s="68" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="E10" s="69">
         <v>27956</v>
       </c>
       <c r="H10" s="37" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="I10" s="72"/>
       <c r="J10" s="73">
@@ -4251,10 +4254,10 @@
         <v>6</v>
       </c>
       <c r="C11" s="67" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D11" s="68" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="E11" s="69">
         <v>27443</v>
@@ -4266,10 +4269,10 @@
         <v>7</v>
       </c>
       <c r="C12" s="67" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D12" s="68" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="E12" s="69">
         <v>27274</v>
@@ -4281,10 +4284,10 @@
         <v>8</v>
       </c>
       <c r="C13" s="67" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D13" s="68" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="E13" s="69">
         <v>21411</v>
@@ -4298,13 +4301,13 @@
     </row>
     <row r="16" spans="1:13" ht="18">
       <c r="C16" s="71" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D16" s="70">
         <v>3</v>
       </c>
       <c r="H16" s="71" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="I16" s="70">
         <v>25250</v>
@@ -4316,23 +4319,23 @@
     </row>
     <row r="18" spans="3:9" ht="21.75" customHeight="1">
       <c r="C18" s="40" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D18" s="50"/>
       <c r="H18" s="71" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="I18" s="50"/>
     </row>
     <row r="19" spans="3:9" ht="21.75" customHeight="1">
       <c r="C19" s="40" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D19" s="50"/>
     </row>
     <row r="20" spans="3:9" ht="21.75" customHeight="1">
       <c r="C20" s="40" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="D20" s="51"/>
     </row>
@@ -4354,7 +4357,7 @@
   <sheetPr published="0"/>
   <dimension ref="A1:M25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
@@ -4366,13 +4369,13 @@
   <sheetData>
     <row r="1" spans="1:13" s="62" customFormat="1" ht="32.25" customHeight="1">
       <c r="A1" s="61" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="62" customFormat="1" ht="24" customHeight="1">
       <c r="A2" s="61"/>
       <c r="B2" s="63" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="M2" s="46"/>
     </row>
@@ -4382,27 +4385,27 @@
     </row>
     <row r="4" spans="1:13" ht="30.95" customHeight="1">
       <c r="C4" s="66" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D4" s="66" t="s">
+        <v>78</v>
+      </c>
+      <c r="E4" s="66" t="s">
+        <v>79</v>
+      </c>
+      <c r="F4" s="66" t="s">
         <v>80</v>
       </c>
-      <c r="E4" s="66" t="s">
+      <c r="G4" s="66" t="s">
         <v>81</v>
       </c>
-      <c r="F4" s="66" t="s">
+      <c r="H4" s="66" t="s">
         <v>82</v>
-      </c>
-      <c r="G4" s="66" t="s">
-        <v>83</v>
-      </c>
-      <c r="H4" s="66" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="16.5" customHeight="1">
       <c r="B5" s="66" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C5" s="52">
         <v>508</v>
@@ -4425,7 +4428,7 @@
     </row>
     <row r="6" spans="1:13" ht="16.5" customHeight="1">
       <c r="B6" s="66" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C6" s="52">
         <v>4272</v>
@@ -4448,21 +4451,21 @@
     </row>
     <row r="9" spans="1:13">
       <c r="C9" s="74" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D9" s="47" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:13">
       <c r="C10" s="74" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="D10" s="53"/>
     </row>
     <row r="11" spans="1:13">
       <c r="C11" s="74" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D11" s="53"/>
     </row>
@@ -4471,24 +4474,24 @@
     </row>
     <row r="17" spans="2:6" ht="15">
       <c r="B17" s="66" t="s">
+        <v>85</v>
+      </c>
+      <c r="C17" s="54" t="s">
         <v>87</v>
       </c>
-      <c r="C17" s="54" t="s">
+      <c r="D17" s="54" t="s">
+        <v>88</v>
+      </c>
+      <c r="E17" s="54" t="s">
         <v>89</v>
       </c>
-      <c r="D17" s="54" t="s">
+      <c r="F17" s="54" t="s">
         <v>90</v>
-      </c>
-      <c r="E17" s="54" t="s">
-        <v>91</v>
-      </c>
-      <c r="F17" s="54" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="18" spans="2:6" ht="15">
       <c r="B18" s="66" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C18" s="53"/>
       <c r="D18" s="53"/>
@@ -4497,7 +4500,7 @@
     </row>
     <row r="19" spans="2:6" ht="15">
       <c r="B19" s="66" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C19" s="76">
         <v>15</v>
@@ -4514,7 +4517,7 @@
     </row>
     <row r="21" spans="2:6">
       <c r="C21" s="74" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="D21" s="75">
         <v>48</v>
@@ -4522,7 +4525,7 @@
     </row>
     <row r="22" spans="2:6">
       <c r="C22" s="74" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="D22" s="55"/>
     </row>
@@ -4556,13 +4559,13 @@
   <sheetData>
     <row r="1" spans="1:13" s="62" customFormat="1" ht="32.25" customHeight="1">
       <c r="A1" s="61" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="2" spans="1:13" s="62" customFormat="1" ht="24" customHeight="1">
       <c r="A2" s="61"/>
       <c r="B2" s="97" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="M2" s="46"/>
     </row>
@@ -4573,13 +4576,13 @@
     </row>
     <row r="4" spans="1:13" ht="15">
       <c r="B4" s="66" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="C4" s="66" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="D4" s="66" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="5" spans="1:13" ht="20.25" customHeight="1">
@@ -4590,7 +4593,7 @@
         <v>612</v>
       </c>
       <c r="D5" s="81" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
     </row>
     <row r="6" spans="1:13" ht="20.25" customHeight="1">
@@ -4601,7 +4604,7 @@
         <v>1808</v>
       </c>
       <c r="D6" s="81" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="20.25" customHeight="1">
@@ -4612,7 +4615,7 @@
         <v>808</v>
       </c>
       <c r="D7" s="81" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="8" spans="1:13" ht="20.25" customHeight="1">
@@ -4623,7 +4626,7 @@
         <v>1811.96</v>
       </c>
       <c r="D8" s="81" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="9" spans="1:13" ht="20.25" customHeight="1">
@@ -4634,7 +4637,7 @@
         <v>24.66</v>
       </c>
       <c r="D9" s="81" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="20.25" customHeight="1">
@@ -4645,7 +4648,7 @@
         <v>219.45</v>
       </c>
       <c r="D10" s="81" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="11" spans="1:13" ht="20.25" customHeight="1">
@@ -4656,7 +4659,7 @@
         <v>63</v>
       </c>
       <c r="D11" s="81" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
     </row>
     <row r="12" spans="1:13" ht="20.25" customHeight="1">
@@ -4667,7 +4670,7 @@
         <v>32.200000000000003</v>
       </c>
       <c r="D12" s="81" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:13" ht="20.25" customHeight="1">
@@ -4678,7 +4681,7 @@
         <v>297.07</v>
       </c>
       <c r="D13" s="81" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="14" spans="1:13" ht="20.25" customHeight="1">
@@ -4689,7 +4692,7 @@
         <v>1240</v>
       </c>
       <c r="D14" s="81" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
     </row>
     <row r="15" spans="1:13" ht="20.25" customHeight="1">
@@ -4700,7 +4703,7 @@
         <v>460</v>
       </c>
       <c r="D15" s="81" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="G15" s="77"/>
       <c r="H15" s="78"/>
@@ -4713,10 +4716,10 @@
     </row>
     <row r="17" spans="2:9">
       <c r="C17" s="24" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D17" s="24" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="F17" s="78"/>
       <c r="G17" s="78"/>
@@ -4724,14 +4727,14 @@
     </row>
     <row r="18" spans="2:9" ht="21.75" customHeight="1">
       <c r="B18" s="29" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="31"/>
     </row>
     <row r="20" spans="2:9" ht="24" customHeight="1">
       <c r="B20" s="29" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="C20" s="30"/>
       <c r="D20" s="31"/>
@@ -4751,10 +4754,10 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr published="0"/>
-  <dimension ref="A1:N32"/>
+  <dimension ref="A1:N33"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -4769,7 +4772,7 @@
   <sheetData>
     <row r="1" spans="1:14" s="62" customFormat="1" ht="32.25" customHeight="1">
       <c r="A1" s="61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="B1" s="39"/>
       <c r="F1" s="39"/>
@@ -4777,280 +4780,285 @@
     <row r="2" spans="1:14" s="62" customFormat="1" ht="24" customHeight="1">
       <c r="A2" s="87"/>
       <c r="B2" s="97" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="F2" s="39"/>
       <c r="L2" s="46"/>
     </row>
     <row r="3" spans="1:14" ht="14.25">
       <c r="B3" s="97" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="4" spans="1:14" ht="12.95" customHeight="1">
-      <c r="B4" s="86"/>
-      <c r="N4" s="59"/>
-    </row>
-    <row r="5" spans="1:14" ht="29.25" customHeight="1">
-      <c r="B5" s="66" t="s">
-        <v>127</v>
-      </c>
-      <c r="C5" s="66" t="s">
-        <v>121</v>
-      </c>
-      <c r="D5" s="66" t="s">
         <v>158</v>
       </c>
-      <c r="E5" s="66" t="s">
-        <v>157</v>
-      </c>
-      <c r="F5" s="66" t="s">
+    </row>
+    <row r="4" spans="1:14" ht="14.25">
+      <c r="B4" s="97" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" ht="12.95" customHeight="1">
+      <c r="B5" s="86"/>
+      <c r="N5" s="59"/>
+    </row>
+    <row r="6" spans="1:14" ht="29.25" customHeight="1">
+      <c r="B6" s="66" t="s">
+        <v>125</v>
+      </c>
+      <c r="C6" s="66" t="s">
+        <v>119</v>
+      </c>
+      <c r="D6" s="66" t="s">
         <v>156</v>
       </c>
-      <c r="G5" s="60"/>
-    </row>
-    <row r="6" spans="1:14">
-      <c r="B6" s="54">
-        <v>1</v>
-      </c>
-      <c r="C6" s="82">
-        <v>11200</v>
-      </c>
-      <c r="D6" s="1">
-        <v>135</v>
-      </c>
-      <c r="E6" s="84"/>
-      <c r="F6" s="85"/>
+      <c r="E6" s="66" t="s">
+        <v>155</v>
+      </c>
+      <c r="F6" s="66" t="s">
+        <v>154</v>
+      </c>
+      <c r="G6" s="60"/>
     </row>
     <row r="7" spans="1:14">
       <c r="B7" s="54">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C7" s="82">
-        <v>26900</v>
+        <v>11200</v>
       </c>
       <c r="D7" s="1">
-        <v>362</v>
-      </c>
-      <c r="E7" s="1"/>
-      <c r="F7" s="1"/>
+        <v>135</v>
+      </c>
+      <c r="E7" s="84"/>
+      <c r="F7" s="85"/>
     </row>
     <row r="8" spans="1:14">
       <c r="B8" s="54">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C8" s="82">
-        <v>130000</v>
-      </c>
-      <c r="D8" s="54">
-        <v>288</v>
+        <v>26900</v>
+      </c>
+      <c r="D8" s="1">
+        <v>362</v>
       </c>
       <c r="E8" s="1"/>
       <c r="F8" s="1"/>
     </row>
     <row r="9" spans="1:14">
       <c r="B9" s="54">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C9" s="82">
-        <v>122000</v>
+        <v>130000</v>
       </c>
       <c r="D9" s="54">
-        <v>378</v>
+        <v>288</v>
       </c>
       <c r="E9" s="1"/>
       <c r="F9" s="1"/>
     </row>
     <row r="10" spans="1:14">
       <c r="B10" s="54">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C10" s="82">
-        <v>4000</v>
+        <v>122000</v>
       </c>
       <c r="D10" s="54">
-        <v>160</v>
+        <v>378</v>
       </c>
       <c r="E10" s="1"/>
       <c r="F10" s="1"/>
     </row>
     <row r="11" spans="1:14">
       <c r="B11" s="54">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C11" s="82">
-        <v>47000</v>
+        <v>4000</v>
       </c>
       <c r="D11" s="54">
-        <v>180</v>
+        <v>160</v>
       </c>
       <c r="E11" s="1"/>
       <c r="F11" s="1"/>
     </row>
     <row r="12" spans="1:14">
       <c r="B12" s="54">
-        <v>7</v>
-      </c>
-      <c r="C12" s="83">
-        <v>43000</v>
+        <v>6</v>
+      </c>
+      <c r="C12" s="82">
+        <v>47000</v>
       </c>
       <c r="D12" s="54">
-        <v>150</v>
+        <v>180</v>
       </c>
       <c r="E12" s="1"/>
       <c r="F12" s="1"/>
     </row>
     <row r="13" spans="1:14">
       <c r="B13" s="54">
-        <v>8</v>
-      </c>
-      <c r="C13" s="82">
-        <v>473000</v>
+        <v>7</v>
+      </c>
+      <c r="C13" s="83">
+        <v>43000</v>
       </c>
       <c r="D13" s="54">
-        <v>200</v>
+        <v>150</v>
       </c>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
     </row>
     <row r="14" spans="1:14">
       <c r="B14" s="54">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C14" s="82">
-        <v>8500</v>
+        <v>473000</v>
       </c>
       <c r="D14" s="54">
-        <v>170</v>
+        <v>200</v>
       </c>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
     </row>
     <row r="15" spans="1:14">
       <c r="B15" s="54">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C15" s="82">
-        <v>42000</v>
+        <v>8500</v>
       </c>
       <c r="D15" s="54">
-        <v>220</v>
+        <v>170</v>
       </c>
       <c r="E15" s="1"/>
       <c r="F15" s="1"/>
     </row>
     <row r="16" spans="1:14">
       <c r="B16" s="54">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C16" s="82">
-        <v>19500</v>
+        <v>42000</v>
       </c>
       <c r="D16" s="54">
-        <v>150</v>
+        <v>220</v>
       </c>
       <c r="E16" s="1"/>
       <c r="F16" s="1"/>
     </row>
     <row r="17" spans="1:6">
       <c r="B17" s="54">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C17" s="82">
-        <v>42000</v>
+        <v>19500</v>
       </c>
       <c r="D17" s="54">
-        <v>91</v>
+        <v>150</v>
       </c>
       <c r="E17" s="1"/>
       <c r="F17" s="1"/>
     </row>
     <row r="18" spans="1:6">
       <c r="B18" s="54">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C18" s="82">
-        <v>23200</v>
+        <v>42000</v>
       </c>
       <c r="D18" s="54">
-        <v>200</v>
+        <v>91</v>
       </c>
       <c r="E18" s="1"/>
       <c r="F18" s="1"/>
     </row>
     <row r="19" spans="1:6">
       <c r="B19" s="54">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C19" s="82">
-        <v>61000</v>
+        <v>23200</v>
       </c>
       <c r="D19" s="54">
-        <v>110</v>
+        <v>200</v>
       </c>
       <c r="E19" s="1"/>
       <c r="F19" s="1"/>
     </row>
     <row r="20" spans="1:6">
       <c r="B20" s="54">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C20" s="82">
-        <v>62900</v>
+        <v>61000</v>
       </c>
       <c r="D20" s="54">
-        <v>147</v>
+        <v>110</v>
       </c>
       <c r="E20" s="1"/>
       <c r="F20" s="1"/>
     </row>
     <row r="21" spans="1:6">
       <c r="B21" s="54">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C21" s="82">
-        <v>56300</v>
+        <v>62900</v>
       </c>
       <c r="D21" s="54">
-        <v>51</v>
+        <v>147</v>
       </c>
       <c r="E21" s="1"/>
       <c r="F21" s="1"/>
     </row>
     <row r="22" spans="1:6">
       <c r="B22" s="54">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C22" s="82">
-        <v>83299</v>
+        <v>56300</v>
       </c>
       <c r="D22" s="54">
-        <v>45</v>
+        <v>51</v>
       </c>
       <c r="E22" s="1"/>
       <c r="F22" s="1"/>
     </row>
     <row r="23" spans="1:6">
       <c r="B23" s="54">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C23" s="82">
-        <v>43000</v>
+        <v>83299</v>
       </c>
       <c r="D23" s="54">
-        <v>465</v>
+        <v>45</v>
       </c>
       <c r="E23" s="1"/>
       <c r="F23" s="1"/>
     </row>
-    <row r="29" spans="1:6">
-      <c r="A29" s="45"/>
-    </row>
-    <row r="31" spans="1:6">
-      <c r="A31" s="45"/>
+    <row r="24" spans="1:6">
+      <c r="B24" s="54">
+        <v>18</v>
+      </c>
+      <c r="C24" s="82">
+        <v>43000</v>
+      </c>
+      <c r="D24" s="54">
+        <v>465</v>
+      </c>
+      <c r="E24" s="1"/>
+      <c r="F24" s="1"/>
+    </row>
+    <row r="30" spans="1:6">
+      <c r="A30" s="45"/>
     </row>
     <row r="32" spans="1:6">
       <c r="A32" s="45"/>
+    </row>
+    <row r="33" spans="1:1">
+      <c r="A33" s="45"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -5082,7 +5090,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="62" customFormat="1" ht="32.25" customHeight="1">
       <c r="A1" s="61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C1" s="39"/>
       <c r="G1" s="39"/>
@@ -5090,21 +5098,21 @@
     <row r="2" spans="1:15" s="62" customFormat="1" ht="24" customHeight="1">
       <c r="A2" s="87"/>
       <c r="B2" s="97" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G2" s="39"/>
       <c r="M2" s="46"/>
     </row>
     <row r="3" spans="1:15" customFormat="1">
       <c r="B3" s="97" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C3" s="4"/>
       <c r="G3" s="3"/>
     </row>
     <row r="4" spans="1:15" customFormat="1">
       <c r="B4" s="97" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C4" s="4"/>
       <c r="G4" s="3"/>
@@ -5116,7 +5124,7 @@
     </row>
     <row r="6" spans="1:15" ht="29.25" customHeight="1">
       <c r="B6" s="142" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C6" s="143"/>
       <c r="D6" s="143"/>
@@ -5127,11 +5135,11 @@
     </row>
     <row r="7" spans="1:15" ht="30" customHeight="1">
       <c r="B7" s="144" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C7" s="146"/>
       <c r="D7" s="144" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="E7" s="145"/>
       <c r="F7" s="145"/>
@@ -5144,21 +5152,21 @@
     </row>
     <row r="9" spans="1:15">
       <c r="B9" s="32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="K9" s="88"/>
     </row>
     <row r="10" spans="1:15">
       <c r="B10" s="33" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D10" s="6" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="B11" s="5" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D11" s="34">
         <v>6</v>
@@ -5166,31 +5174,31 @@
     </row>
     <row r="12" spans="1:15" ht="15.75">
       <c r="B12" s="5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D12" s="35"/>
     </row>
     <row r="14" spans="1:15" ht="25.5" customHeight="1">
       <c r="B14" s="66" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="66" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="66" t="s">
         <v>33</v>
-      </c>
-      <c r="C14" s="66" t="s">
-        <v>34</v>
-      </c>
-      <c r="D14" s="66" t="s">
-        <v>35</v>
       </c>
       <c r="E14" s="66" t="s">
         <v>0</v>
       </c>
       <c r="F14" s="66" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="G14" s="66" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H14" s="66" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="15.75">
@@ -5198,7 +5206,7 @@
         <v>43344</v>
       </c>
       <c r="C15" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D15" s="6">
         <v>162</v>
@@ -5217,7 +5225,7 @@
         <v>43349</v>
       </c>
       <c r="C16" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D16" s="6">
         <v>74</v>
@@ -5232,7 +5240,7 @@
         <v>43350</v>
       </c>
       <c r="C17" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D17" s="6">
         <v>135</v>
@@ -5251,7 +5259,7 @@
         <v>43357</v>
       </c>
       <c r="C18" s="20" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D18" s="6">
         <v>70</v>
@@ -5266,7 +5274,7 @@
         <v>43358</v>
       </c>
       <c r="C19" s="20" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D19" s="6">
         <v>162</v>
@@ -5283,7 +5291,7 @@
         <v>43360</v>
       </c>
       <c r="C20" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D20" s="6">
         <v>154</v>
@@ -5302,7 +5310,7 @@
         <v>43364</v>
       </c>
       <c r="C21" s="20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D21" s="6">
         <v>243</v>
@@ -5319,7 +5327,7 @@
         <v>43367</v>
       </c>
       <c r="C22" s="20" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D22" s="6">
         <v>135</v>
@@ -5336,7 +5344,7 @@
         <v>43372</v>
       </c>
       <c r="C23" s="21" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D23" s="13">
         <v>150</v>
@@ -5351,7 +5359,7 @@
     <row r="24" spans="2:8" ht="23.25" customHeight="1">
       <c r="B24" s="7"/>
       <c r="G24" s="89" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="H24" s="35"/>
     </row>
@@ -5414,18 +5422,18 @@
     </row>
     <row r="4" spans="1:4" ht="51.75" customHeight="1">
       <c r="B4" s="144" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C4" s="145"/>
       <c r="D4" s="146"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1">
       <c r="B5" s="144" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C5" s="146"/>
       <c r="D5" s="66" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:4" s="90" customFormat="1" ht="23.25" customHeight="1">
@@ -5433,7 +5441,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="92" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D6" s="94">
         <v>0.439</v>
@@ -5444,7 +5452,7 @@
         <v>5</v>
       </c>
       <c r="C7" s="92" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D7" s="94">
         <v>0.505</v>
@@ -5455,7 +5463,7 @@
         <v>8</v>
       </c>
       <c r="C8" s="92" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D8" s="94">
         <v>0.57199999999999995</v>
@@ -5467,7 +5475,7 @@
         <v>10</v>
       </c>
       <c r="C9" s="92" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D9" s="94">
         <v>0.61399999999999999</v>
@@ -5478,7 +5486,7 @@
         <v>12</v>
       </c>
       <c r="C10" s="92" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D10" s="94">
         <v>0.65600000000000003</v>
@@ -5525,7 +5533,7 @@
   <sheetData>
     <row r="1" spans="1:15" s="62" customFormat="1" ht="32.25" customHeight="1">
       <c r="A1" s="61" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C1" s="39"/>
       <c r="G1" s="39"/>
@@ -5533,14 +5541,14 @@
     <row r="2" spans="1:15" s="62" customFormat="1" ht="24" customHeight="1">
       <c r="A2" s="87"/>
       <c r="B2" s="97" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="G2" s="39"/>
       <c r="M2" s="46"/>
     </row>
     <row r="3" spans="1:15" customFormat="1" ht="15">
       <c r="B3" s="97" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C3" s="4"/>
       <c r="G3" s="3"/>
@@ -5552,69 +5560,69 @@
     </row>
     <row r="5" spans="1:15" ht="30">
       <c r="B5" s="66" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C5" s="66" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D5" s="66" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E5" s="66" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="16.5" customHeight="1">
       <c r="B6" s="58" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C6" s="95">
         <v>86000</v>
       </c>
       <c r="D6" s="54" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E6" s="96"/>
       <c r="G6" s="144" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="H6" s="145"/>
       <c r="I6" s="146"/>
     </row>
     <row r="7" spans="1:15" ht="16.5" customHeight="1">
       <c r="B7" s="58" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C7" s="95">
         <v>78000</v>
       </c>
       <c r="D7" s="54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E7" s="43"/>
       <c r="G7" s="54" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H7" s="54" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I7" s="54" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="8" spans="1:15" ht="16.5" customHeight="1">
       <c r="B8" s="58" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C8" s="95">
         <v>40000</v>
       </c>
       <c r="D8" s="54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E8" s="43"/>
       <c r="G8" s="56" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="H8" s="96"/>
       <c r="I8" s="57">
@@ -5623,17 +5631,17 @@
     </row>
     <row r="9" spans="1:15" ht="16.5" customHeight="1">
       <c r="B9" s="58" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C9" s="95">
         <v>125000</v>
       </c>
       <c r="D9" s="54" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E9" s="43"/>
       <c r="G9" s="43" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="H9" s="96"/>
       <c r="I9" s="57">
@@ -5642,17 +5650,17 @@
     </row>
     <row r="10" spans="1:15" ht="16.5" customHeight="1">
       <c r="B10" s="58" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C10" s="95">
         <v>68000</v>
       </c>
       <c r="D10" s="54" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E10" s="43"/>
       <c r="G10" s="56" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="H10" s="96"/>
       <c r="I10" s="57">
@@ -5661,17 +5669,17 @@
     </row>
     <row r="11" spans="1:15" ht="16.5" customHeight="1">
       <c r="B11" s="58" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C11" s="95">
         <v>35000</v>
       </c>
       <c r="D11" s="54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E11" s="43"/>
       <c r="G11" s="56" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="H11" s="96"/>
       <c r="I11" s="57">
@@ -5680,67 +5688,67 @@
     </row>
     <row r="12" spans="1:15" ht="16.5" customHeight="1">
       <c r="B12" s="58" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C12" s="95">
         <v>50000</v>
       </c>
       <c r="D12" s="54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E12" s="43"/>
     </row>
     <row r="13" spans="1:15" ht="16.5" customHeight="1">
       <c r="B13" s="58" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C13" s="95">
         <v>79000</v>
       </c>
       <c r="D13" s="54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E13" s="43"/>
       <c r="G13" s="144" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="H13" s="145"/>
       <c r="I13" s="146"/>
     </row>
     <row r="14" spans="1:15" ht="16.5" customHeight="1">
       <c r="B14" s="58" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="C14" s="95">
         <v>41000</v>
       </c>
       <c r="D14" s="54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E14" s="43"/>
       <c r="G14" s="54" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="H14" s="54" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="I14" s="54" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="15" spans="1:15" ht="16.5" customHeight="1">
       <c r="B15" s="58" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C15" s="95">
         <v>75000</v>
       </c>
       <c r="D15" s="54" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="E15" s="43"/>
       <c r="G15" s="56" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="H15" s="96"/>
       <c r="I15" s="57">
@@ -5749,17 +5757,17 @@
     </row>
     <row r="16" spans="1:15" ht="16.5" customHeight="1">
       <c r="B16" s="58" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C16" s="95">
         <v>198500</v>
       </c>
       <c r="D16" s="54" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E16" s="43"/>
       <c r="G16" s="56" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="H16" s="96"/>
       <c r="I16" s="57">
@@ -5768,17 +5776,17 @@
     </row>
     <row r="17" spans="2:9" ht="16.5" customHeight="1">
       <c r="B17" s="58" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C17" s="95">
         <v>138000</v>
       </c>
       <c r="D17" s="54" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E17" s="43"/>
       <c r="G17" s="56" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="H17" s="96"/>
       <c r="I17" s="57">
@@ -5787,13 +5795,13 @@
     </row>
     <row r="18" spans="2:9" ht="16.5" customHeight="1">
       <c r="B18" s="58" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C18" s="95">
         <v>280000</v>
       </c>
       <c r="D18" s="54" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E18" s="43"/>
     </row>

</xml_diff>

<commit_message>
Filtres et mises en forme conditionnelles
</commit_message>
<xml_diff>
--- a/FonctionsDeRecherche.xlsx
+++ b/FonctionsDeRecherche.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4506"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="28025"/>
   <workbookPr autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Sophie\Documents\CampusDiderot\2024-25\CI\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A822B474-3B36-43B8-8FEA-C9999728E8C1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="16440" tabRatio="557" firstSheet="1" activeTab="1"/>
+    <workbookView xWindow="7530" yWindow="0" windowWidth="20880" windowHeight="15645" tabRatio="557" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RECHERCHEV" sheetId="9882" r:id="rId1"/>
@@ -39,7 +45,7 @@
     <definedName name="Vehicules">[1]Véhicules!$N$3:$AA$11</definedName>
     <definedName name="zaa">[1]Classement!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:ArchID Flags="2"/>
@@ -49,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="277" uniqueCount="213">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="281" uniqueCount="217">
   <si>
     <t>Frais transport</t>
   </si>
@@ -689,9 +695,6 @@
     <t>MARSEILLE</t>
   </si>
   <si>
-    <t>Excel recherche dans la première colonne du tableau la plus grande des bornes strictement inférieure à la valeur qu'on lui fournit.</t>
-  </si>
-  <si>
     <t>Exemple : recherche par valeur exacte (type=FAUX)</t>
   </si>
   <si>
@@ -732,12 +735,48 @@
   </si>
   <si>
     <t>De 24 873 à 66 678 €</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Excel recherche dans la </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color rgb="FFFF0000"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>première colonne du tableau</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> la plus grande des bornes strictement inférieure à la valeur qu'on lui fournit.</t>
+    </r>
+  </si>
+  <si>
+    <t>1er :tableau de données : B6:D11</t>
+  </si>
+  <si>
+    <t>2eme: quelle colonne se trouve l'info qui m'intéresse : 2</t>
+  </si>
+  <si>
+    <t>1er : quelle est la donnée que Excel doit trouver dans le tableau : LEJEUNE</t>
+  </si>
+  <si>
+    <t>3eme : est-ce que la donnee n'est pas exactement dans le tableau ? FAUX</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="9">
     <numFmt numFmtId="8" formatCode="#,##0.00\ &quot;€&quot;;[Red]\-#,##0.00\ &quot;€&quot;"/>
     <numFmt numFmtId="44" formatCode="_-* #,##0.00\ &quot;€&quot;_-;\-* #,##0.00\ &quot;€&quot;_-;_-* &quot;-&quot;??\ &quot;€&quot;_-;_-@_-"/>
@@ -749,7 +788,7 @@
     <numFmt numFmtId="169" formatCode="General_)"/>
     <numFmt numFmtId="170" formatCode="#,##0.00\ &quot;€&quot;"/>
   </numFmts>
-  <fonts count="42">
+  <fonts count="43">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -999,6 +1038,13 @@
       <b/>
       <sz val="10"/>
       <color theme="0"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1667,7 +1713,6 @@
     <xf numFmtId="0" fontId="1" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="4" xfId="14" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1698,38 +1743,39 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="19" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="30">
-    <cellStyle name="Comma [0]" xfId="1"/>
-    <cellStyle name="Currency [0]" xfId="2"/>
-    <cellStyle name="Currency_Macro1" xfId="3"/>
-    <cellStyle name="Dezimal [0]" xfId="4"/>
-    <cellStyle name="Euro" xfId="5"/>
-    <cellStyle name="Euro_exos" xfId="6"/>
-    <cellStyle name="Euro_TD Fx Recherche" xfId="7"/>
-    <cellStyle name="heure" xfId="8"/>
-    <cellStyle name="Milliers_TD 3 Fx Recherche et SI" xfId="9"/>
-    <cellStyle name="Modif" xfId="10"/>
-    <cellStyle name="Monétaire [+]" xfId="11"/>
-    <cellStyle name="nom" xfId="12"/>
-    <cellStyle name="nor1" xfId="13"/>
-    <cellStyle name="nor1 2" xfId="28"/>
+    <cellStyle name="Comma [0]" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="Currency [0]" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="Currency_Macro1" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="Dezimal [0]" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="Euro" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="Euro_exos" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="Euro_TD Fx Recherche" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="heure" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="Milliers_TD 3 Fx Recherche et SI" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Modif" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Monétaire [+]" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="nom" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="nor1" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="nor1 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 4" xfId="26"/>
-    <cellStyle name="Normal_fonction recherche" xfId="14"/>
-    <cellStyle name="Normal_Fonctions de base" xfId="15"/>
-    <cellStyle name="Normal_Fonctions de recherche (3)" xfId="16"/>
-    <cellStyle name="Normal_FORMULE2" xfId="27"/>
-    <cellStyle name="Normal_Recherche et base" xfId="17"/>
-    <cellStyle name="Normal_SDIS perf" xfId="18"/>
-    <cellStyle name="Normal_TD Fx Recherche" xfId="19"/>
-    <cellStyle name="poste" xfId="20"/>
-    <cellStyle name="Pourcentage 2" xfId="29"/>
-    <cellStyle name="Standard_Iterative Kostenberechnung" xfId="21"/>
-    <cellStyle name="Titel" xfId="22"/>
-    <cellStyle name="titre" xfId="23"/>
-    <cellStyle name="Titre1" xfId="24"/>
-    <cellStyle name="Währung [0]" xfId="25"/>
+    <cellStyle name="Normal 4" xfId="26" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="Normal_fonction recherche" xfId="14" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="Normal_Fonctions de base" xfId="15" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="Normal_Fonctions de recherche (3)" xfId="16" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="Normal_FORMULE2" xfId="27" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="Normal_Recherche et base" xfId="17" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="Normal_SDIS perf" xfId="18" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="Normal_TD Fx Recherche" xfId="19" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="poste" xfId="20" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="Pourcentage 2" xfId="29" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="Standard_Iterative Kostenberechnung" xfId="21" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="Titel" xfId="22" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="titre" xfId="23" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Titre1" xfId="24" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="Währung [0]" xfId="25" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2"/>
@@ -1780,7 +1826,7 @@
         <xdr:cNvPr id="56" name="Image 55">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0500-000038000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0500-000038000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1829,7 +1875,7 @@
         <xdr:cNvPr id="15363" name="Line 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0B00-0000033C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-0000033C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1856,7 +1902,7 @@
         </a:ln>
         <a:extLst>
           <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
-            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:noFill/>
             </a14:hiddenFill>
           </a:ext>
@@ -1883,7 +1929,7 @@
         <xdr:cNvPr id="15365" name="AutoShape 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0B00-0000053C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-0000053C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2029,7 +2075,7 @@
         <xdr:cNvPr id="15366" name="AutoShape 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0B00-0000063C0000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0B00-0000063C0000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2157,11 +2203,61 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+      <xdr:twoCellAnchor>
+        <xdr:from>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>9</xdr:row>
+          <xdr:rowOff>28575</xdr:rowOff>
+        </xdr:from>
+        <xdr:to>
+          <xdr:col>0</xdr:col>
+          <xdr:colOff>0</xdr:colOff>
+          <xdr:row>10</xdr:row>
+          <xdr:rowOff>0</xdr:rowOff>
+        </xdr:to>
+        <xdr:sp macro="" textlink="">
+          <xdr:nvSpPr>
+            <xdr:cNvPr id="15361" name="Spinner 1" hidden="1">
+              <a:extLst>
+                <a:ext uri="{63B3BB69-23CF-44E3-9099-C40C66FF867C}">
+                  <a14:compatExt spid="_x0000_s15361"/>
+                </a:ext>
+                <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                  <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A511C975-6051-363E-B7AF-6203F795C6D1}"/>
+                </a:ext>
+              </a:extLst>
+            </xdr:cNvPr>
+            <xdr:cNvSpPr/>
+          </xdr:nvSpPr>
+          <xdr:spPr bwMode="auto">
+            <a:xfrm>
+              <a:off x="0" y="0"/>
+              <a:ext cx="0" cy="0"/>
+            </a:xfrm>
+            <a:prstGeom prst="rect">
+              <a:avLst/>
+            </a:prstGeom>
+            <a:noFill/>
+            <a:ln w="9525">
+              <a:miter lim="800000"/>
+              <a:headEnd/>
+              <a:tailEnd/>
+            </a:ln>
+          </xdr:spPr>
+        </xdr:sp>
+        <xdr:clientData/>
+      </xdr:twoCellAnchor>
+    </mc:Choice>
+    <mc:Fallback/>
+  </mc:AlternateContent>
 </xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xxl21="http://schemas.microsoft.com/office/spreadsheetml/2021/extlinks2021" mc:Ignorable="x14 xxl21">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="Fonction RECHERCHEV"/>
@@ -2998,7 +3094,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -3040,7 +3136,7 @@
         <a:effectLst/>
         <a:extLst>
           <a:ext uri="{AF507438-7753-43E0-B8FC-AC1667EBCBE1}">
-            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" xmlns="">
+            <a14:hiddenEffects xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
               <a:effectLst>
                 <a:outerShdw dist="35921" dir="2700000" algn="ctr" rotWithShape="0">
                   <a:srgbClr val="808080"/>
@@ -3059,12 +3155,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr published="0"/>
   <dimension ref="A1:H22"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J19" sqref="J19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G27" sqref="G27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75"/>
@@ -3099,7 +3195,7 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="14.25">
-      <c r="B6" s="139" t="s">
+      <c r="B6" s="138" t="s">
         <v>44</v>
       </c>
       <c r="C6" s="132" t="s">
@@ -3109,11 +3205,11 @@
         <v>2</v>
       </c>
       <c r="F6" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15" customHeight="1">
-      <c r="B7" s="139" t="s">
+      <c r="B7" s="138" t="s">
         <v>46</v>
       </c>
       <c r="C7" s="132" t="s">
@@ -3126,11 +3222,11 @@
         <v>122</v>
       </c>
       <c r="G7" s="48" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15" customHeight="1">
-      <c r="B8" s="139" t="s">
+      <c r="B8" s="138" t="s">
         <v>48</v>
       </c>
       <c r="C8" s="132" t="s">
@@ -3142,10 +3238,13 @@
       <c r="F8" s="66" t="s">
         <v>192</v>
       </c>
-      <c r="G8" s="136"/>
+      <c r="G8" s="136" t="str">
+        <f>VLOOKUP(G7,B6:D11,2,FALSE)</f>
+        <v>NICE</v>
+      </c>
     </row>
     <row r="9" spans="1:7" ht="14.25">
-      <c r="B9" s="139" t="s">
+      <c r="B9" s="138" t="s">
         <v>50</v>
       </c>
       <c r="C9" s="132" t="s">
@@ -3156,7 +3255,7 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="14.25">
-      <c r="B10" s="139" t="s">
+      <c r="B10" s="138" t="s">
         <v>52</v>
       </c>
       <c r="C10" s="132" t="s">
@@ -3165,9 +3264,12 @@
       <c r="D10" s="133">
         <v>7</v>
       </c>
+      <c r="F10" s="45" t="s">
+        <v>215</v>
+      </c>
     </row>
     <row r="11" spans="1:7" ht="14.25">
-      <c r="B11" s="139" t="s">
+      <c r="B11" s="138" t="s">
         <v>57</v>
       </c>
       <c r="C11" s="132" t="s">
@@ -3175,6 +3277,19 @@
       </c>
       <c r="D11" s="133">
         <v>2</v>
+      </c>
+      <c r="F11" s="148" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
+      <c r="F12" s="148" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7">
+      <c r="F13" s="45" t="s">
+        <v>216</v>
       </c>
     </row>
     <row r="15" spans="1:7" s="62" customFormat="1" ht="19.5" customHeight="1">
@@ -3223,7 +3338,7 @@
         <v>25</v>
       </c>
       <c r="F20" s="66" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G20" s="137"/>
     </row>
@@ -3244,8 +3359,8 @@
       <c r="D22" s="133">
         <v>120</v>
       </c>
-      <c r="F22" s="138" t="s">
-        <v>198</v>
+      <c r="F22" s="114" t="s">
+        <v>212</v>
       </c>
     </row>
   </sheetData>
@@ -3260,7 +3375,7 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
   <sheetPr published="0"/>
   <dimension ref="A1:O24"/>
   <sheetViews>
@@ -3317,13 +3432,13 @@
       <c r="O6" s="59"/>
     </row>
     <row r="7" spans="1:15" ht="21" customHeight="1">
-      <c r="B7" s="144" t="s">
+      <c r="B7" s="143" t="s">
         <v>16</v>
       </c>
-      <c r="C7" s="145"/>
-      <c r="D7" s="145"/>
-      <c r="E7" s="145"/>
-      <c r="F7" s="146"/>
+      <c r="C7" s="144"/>
+      <c r="D7" s="144"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="145"/>
     </row>
     <row r="8" spans="1:15" ht="23.25" customHeight="1">
       <c r="B8" s="66" t="s">
@@ -3474,7 +3589,7 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <sheetPr published="0"/>
   <dimension ref="A1:M10"/>
   <sheetViews>
@@ -3494,11 +3609,11 @@
       <c r="M1" s="46"/>
     </row>
     <row r="2" spans="1:13" ht="30" customHeight="1">
-      <c r="B2" s="144" t="s">
+      <c r="B2" s="143" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="145"/>
-      <c r="D2" s="146"/>
+      <c r="C2" s="144"/>
+      <c r="D2" s="145"/>
     </row>
     <row r="3" spans="1:13" ht="27.75" customHeight="1">
       <c r="B3" s="66" t="s">
@@ -3604,7 +3719,7 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0B00-000000000000}">
   <sheetPr published="0"/>
   <dimension ref="A1:Q24"/>
   <sheetViews>
@@ -3654,12 +3769,12 @@
       <c r="Q3"/>
     </row>
     <row r="4" spans="1:17" ht="21.75" customHeight="1">
-      <c r="B4" s="142" t="s">
+      <c r="B4" s="141" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="143"/>
-      <c r="D4" s="143"/>
-      <c r="E4" s="147"/>
+      <c r="C4" s="142"/>
+      <c r="D4" s="142"/>
+      <c r="E4" s="146"/>
       <c r="H4"/>
       <c r="I4"/>
       <c r="J4"/>
@@ -3705,10 +3820,10 @@
     </row>
     <row r="8" spans="1:17" ht="21.75" customHeight="1">
       <c r="B8" s="27"/>
-      <c r="C8" s="148" t="s">
+      <c r="C8" s="147" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="148"/>
+      <c r="D8" s="147"/>
       <c r="E8" s="130"/>
       <c r="H8" s="114"/>
       <c r="I8" s="2"/>
@@ -3917,6 +4032,34 @@
   <headerFooter alignWithMargins="0"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x14">
+      <controls>
+        <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+          <mc:Choice Requires="x14">
+            <control shapeId="15361" r:id="rId3" name="Spinner 1">
+              <controlPr defaultSize="0" autoPict="0">
+                <anchor moveWithCells="1" sizeWithCells="1">
+                  <from>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>9</xdr:row>
+                    <xdr:rowOff>28575</xdr:rowOff>
+                  </from>
+                  <to>
+                    <xdr:col>0</xdr:col>
+                    <xdr:colOff>0</xdr:colOff>
+                    <xdr:row>10</xdr:row>
+                    <xdr:rowOff>0</xdr:rowOff>
+                  </to>
+                </anchor>
+              </controlPr>
+            </control>
+          </mc:Choice>
+        </mc:AlternateContent>
+      </controls>
+    </mc:Choice>
+  </mc:AlternateContent>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="http://schemas.microsoft.com/office/mac/excel/2008/main">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>
@@ -3926,11 +4069,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr published="0"/>
   <dimension ref="A1:O9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
@@ -3952,17 +4095,17 @@
     </row>
     <row r="3" spans="1:15" s="62" customFormat="1" ht="19.5" customHeight="1">
       <c r="A3" s="135" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="4" spans="1:15" s="97" customFormat="1" ht="14.25">
       <c r="A4" s="97" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="6" spans="1:15" ht="21" customHeight="1">
-      <c r="B6" s="141" t="s">
-        <v>206</v>
+      <c r="B6" s="140" t="s">
+        <v>205</v>
       </c>
       <c r="C6" s="49"/>
       <c r="D6" s="49"/>
@@ -3973,7 +4116,7 @@
       <c r="I6" s="49"/>
       <c r="J6" s="49"/>
       <c r="M6" s="66" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="N6" s="66" t="s">
         <v>192</v>
@@ -3984,37 +4127,37 @@
     </row>
     <row r="7" spans="1:15" ht="21" customHeight="1">
       <c r="B7" s="66" t="s">
+        <v>203</v>
+      </c>
+      <c r="C7" s="138" t="s">
+        <v>44</v>
+      </c>
+      <c r="D7" s="138" t="s">
+        <v>46</v>
+      </c>
+      <c r="E7" s="138" t="s">
+        <v>48</v>
+      </c>
+      <c r="F7" s="138" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="138" t="s">
         <v>204</v>
       </c>
-      <c r="C7" s="139" t="s">
-        <v>44</v>
-      </c>
-      <c r="D7" s="139" t="s">
-        <v>46</v>
-      </c>
-      <c r="E7" s="139" t="s">
-        <v>48</v>
-      </c>
-      <c r="F7" s="139" t="s">
-        <v>50</v>
-      </c>
-      <c r="G7" s="139" t="s">
-        <v>205</v>
-      </c>
-      <c r="H7" s="139" t="s">
+      <c r="H7" s="138" t="s">
         <v>57</v>
       </c>
       <c r="I7" s="48" t="s">
+        <v>199</v>
+      </c>
+      <c r="J7" s="48" t="s">
         <v>200</v>
       </c>
-      <c r="J7" s="48" t="s">
-        <v>201</v>
-      </c>
-      <c r="M7" s="139" t="s">
-        <v>205</v>
+      <c r="M7" s="138" t="s">
+        <v>204</v>
       </c>
       <c r="N7" s="134"/>
-      <c r="O7" s="140"/>
+      <c r="O7" s="139"/>
     </row>
     <row r="8" spans="1:15" ht="21" customHeight="1">
       <c r="B8" s="66" t="s">
@@ -4039,10 +4182,10 @@
         <v>197</v>
       </c>
       <c r="I8" s="48" t="s">
+        <v>201</v>
+      </c>
+      <c r="J8" s="48" t="s">
         <v>202</v>
-      </c>
-      <c r="J8" s="48" t="s">
-        <v>203</v>
       </c>
       <c r="M8" s="45"/>
     </row>
@@ -4081,7 +4224,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr published="0"/>
   <dimension ref="A1:M21"/>
   <sheetViews>
@@ -4158,7 +4301,7 @@
         <v>23235</v>
       </c>
       <c r="H6" s="37" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="I6" s="72"/>
       <c r="J6" s="73">
@@ -4221,7 +4364,7 @@
         <v>23483</v>
       </c>
       <c r="H9" s="37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="I9" s="72"/>
       <c r="J9" s="73">
@@ -4353,7 +4496,7 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <sheetPr published="0"/>
   <dimension ref="A1:M25"/>
   <sheetViews>
@@ -4542,7 +4685,7 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
   <sheetPr published="0"/>
   <dimension ref="A1:M20"/>
   <sheetViews>
@@ -4752,7 +4895,7 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <sheetPr published="0"/>
   <dimension ref="A1:N33"/>
   <sheetViews>
@@ -4792,7 +4935,7 @@
     </row>
     <row r="4" spans="1:14" ht="14.25">
       <c r="B4" s="97" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="12.95" customHeight="1">
@@ -5068,7 +5211,7 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <sheetPr published="0"/>
   <dimension ref="A1:O27"/>
   <sheetViews>
@@ -5123,28 +5266,28 @@
       <c r="O5" s="59"/>
     </row>
     <row r="6" spans="1:15" ht="29.25" customHeight="1">
-      <c r="B6" s="142" t="s">
+      <c r="B6" s="141" t="s">
         <v>30</v>
       </c>
-      <c r="C6" s="143"/>
-      <c r="D6" s="143"/>
-      <c r="E6" s="143"/>
-      <c r="F6" s="143"/>
-      <c r="G6" s="143"/>
-      <c r="H6" s="143"/>
+      <c r="C6" s="142"/>
+      <c r="D6" s="142"/>
+      <c r="E6" s="142"/>
+      <c r="F6" s="142"/>
+      <c r="G6" s="142"/>
+      <c r="H6" s="142"/>
     </row>
     <row r="7" spans="1:15" ht="30" customHeight="1">
-      <c r="B7" s="144" t="s">
+      <c r="B7" s="143" t="s">
         <v>59</v>
       </c>
-      <c r="C7" s="146"/>
-      <c r="D7" s="144" t="s">
+      <c r="C7" s="145"/>
+      <c r="D7" s="143" t="s">
         <v>65</v>
       </c>
-      <c r="E7" s="145"/>
-      <c r="F7" s="145"/>
-      <c r="G7" s="145"/>
-      <c r="H7" s="146"/>
+      <c r="E7" s="144"/>
+      <c r="F7" s="144"/>
+      <c r="G7" s="144"/>
+      <c r="H7" s="145"/>
       <c r="K7" s="88"/>
     </row>
     <row r="8" spans="1:15">
@@ -5393,7 +5536,7 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0700-000000000000}">
   <sheetPr published="0"/>
   <dimension ref="A1:D10"/>
   <sheetViews>
@@ -5421,17 +5564,17 @@
       <c r="D3" s="8"/>
     </row>
     <row r="4" spans="1:4" ht="51.75" customHeight="1">
-      <c r="B4" s="144" t="s">
+      <c r="B4" s="143" t="s">
         <v>71</v>
       </c>
-      <c r="C4" s="145"/>
-      <c r="D4" s="146"/>
+      <c r="C4" s="144"/>
+      <c r="D4" s="145"/>
     </row>
     <row r="5" spans="1:4" ht="30" customHeight="1">
-      <c r="B5" s="144" t="s">
+      <c r="B5" s="143" t="s">
         <v>66</v>
       </c>
-      <c r="C5" s="146"/>
+      <c r="C5" s="145"/>
       <c r="D5" s="66" t="s">
         <v>67</v>
       </c>
@@ -5509,7 +5652,7 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <sheetPr published="0"/>
   <dimension ref="A1:O18"/>
   <sheetViews>
@@ -5583,11 +5726,11 @@
         <v>107</v>
       </c>
       <c r="E6" s="96"/>
-      <c r="G6" s="144" t="s">
+      <c r="G6" s="143" t="s">
         <v>163</v>
       </c>
-      <c r="H6" s="145"/>
-      <c r="I6" s="146"/>
+      <c r="H6" s="144"/>
+      <c r="I6" s="145"/>
     </row>
     <row r="7" spans="1:15" ht="16.5" customHeight="1">
       <c r="B7" s="58" t="s">
@@ -5709,11 +5852,11 @@
         <v>108</v>
       </c>
       <c r="E13" s="43"/>
-      <c r="G13" s="144" t="s">
+      <c r="G13" s="143" t="s">
         <v>164</v>
       </c>
-      <c r="H13" s="145"/>
-      <c r="I13" s="146"/>
+      <c r="H13" s="144"/>
+      <c r="I13" s="145"/>
     </row>
     <row r="14" spans="1:15" ht="16.5" customHeight="1">
       <c r="B14" s="58" t="s">

</xml_diff>